<commit_message>
Made another version of dashboard
</commit_message>
<xml_diff>
--- a/Interactive_dashboard/Summary of SAS.xlsx
+++ b/Interactive_dashboard/Summary of SAS.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\NISR\Hackathon2023\Interactive_dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D55FB-7A8A-4391-8FD1-C1C0E1D4F6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D64E8D-C3DC-41B9-90C8-7DFA7E76D222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="12" activeTab="12" xr2:uid="{A4F23BED-4CE7-4605-BABF-D8A624246C5B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" firstSheet="14" activeTab="23" xr2:uid="{A4F23BED-4CE7-4605-BABF-D8A624246C5B}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
     <sheet name="2021" sheetId="2" r:id="rId2"/>
-    <sheet name="d" sheetId="3" r:id="rId3"/>
+    <sheet name="2022" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
@@ -48,14 +48,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="59">
   <si>
     <t>Maize</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Sorghum</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
   </si>
   <si>
     <t>Yams &amp; Taro</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - </t>
   </si>
   <si>
     <t>Banana</t>
@@ -355,13 +349,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -682,7 +676,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,19 +686,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -717,14 +711,12 @@
       <c r="C2" s="2">
         <v>72918</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>33295</v>
@@ -732,14 +724,12 @@
       <c r="C3" s="2">
         <v>136124</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="13"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>14507</v>
@@ -747,14 +737,12 @@
       <c r="C4" s="2">
         <v>15077</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="13"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>4187</v>
@@ -762,14 +750,12 @@
       <c r="C5" s="2">
         <v>8122</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="13"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>190447</v>
@@ -777,14 +763,12 @@
       <c r="C6" s="2">
         <v>192156</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="13"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>89427</v>
@@ -799,7 +783,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>51516</v>
@@ -814,7 +798,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>18058</v>
@@ -822,14 +806,12 @@
       <c r="C9" s="2">
         <v>14565</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="13"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>272500</v>
@@ -837,14 +819,12 @@
       <c r="C10" s="2">
         <v>207635</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>106409</v>
@@ -852,14 +832,12 @@
       <c r="C11" s="2">
         <v>62054</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>39688</v>
@@ -867,14 +845,12 @@
       <c r="C12" s="2">
         <v>30911</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="13"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>126402</v>
@@ -882,14 +858,12 @@
       <c r="C13" s="2">
         <v>114670</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>362199</v>
@@ -904,7 +878,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>10530</v>
@@ -919,7 +893,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>14609</v>
@@ -927,14 +901,12 @@
       <c r="C16" s="2">
         <v>21292</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="13"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>24677</v>
@@ -949,7 +921,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>18246</v>
@@ -964,7 +936,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>7256</v>
@@ -972,9 +944,7 @@
       <c r="C19" s="2">
         <v>7824</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="13"/>
     </row>
   </sheetData>
@@ -988,7 +958,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,19 +968,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1023,14 +993,12 @@
       <c r="C2" s="2">
         <v>1298</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>1268</v>
@@ -1038,14 +1006,12 @@
       <c r="C3" s="2">
         <v>942.2</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>3600</v>
@@ -1053,14 +1019,12 @@
       <c r="C4" s="2">
         <v>4264</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>988</v>
@@ -1068,14 +1032,12 @@
       <c r="C5" s="2">
         <v>1068</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>14056</v>
@@ -1083,14 +1045,12 @@
       <c r="C6" s="2">
         <v>15073</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>7101</v>
@@ -1098,14 +1058,12 @@
       <c r="C7" s="2">
         <v>7232</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>8298</v>
@@ -1113,14 +1071,12 @@
       <c r="C8" s="2">
         <v>8019</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>5911</v>
@@ -1128,14 +1084,12 @@
       <c r="C9" s="2">
         <v>7046</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>10861</v>
@@ -1143,14 +1097,12 @@
       <c r="C10" s="2">
         <v>11781</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>13794</v>
@@ -1158,14 +1110,12 @@
       <c r="C11" s="2">
         <v>18573</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>7927</v>
@@ -1173,14 +1123,12 @@
       <c r="C12" s="2">
         <v>12180</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>9606</v>
@@ -1188,14 +1136,12 @@
       <c r="C13" s="2">
         <v>8398</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>626</v>
@@ -1210,7 +1156,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>753</v>
@@ -1218,14 +1164,12 @@
       <c r="C15" s="2">
         <v>910</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>1598</v>
@@ -1233,14 +1177,12 @@
       <c r="C16" s="2">
         <v>1298</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>1268</v>
@@ -1248,14 +1190,12 @@
       <c r="C17" s="2">
         <v>942.2</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>3600</v>
@@ -1263,14 +1203,12 @@
       <c r="C18" s="2">
         <v>4264</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="16"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>988</v>
@@ -1278,9 +1216,7 @@
       <c r="C19" s="2">
         <v>1068</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>
@@ -1293,7 +1229,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,19 +1239,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1328,14 +1264,12 @@
       <c r="C2" s="2">
         <v>1291</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>1309</v>
@@ -1343,14 +1277,12 @@
       <c r="C3" s="2">
         <v>1010</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>4160</v>
@@ -1358,14 +1290,12 @@
       <c r="C4" s="2">
         <v>4159</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>1018</v>
@@ -1373,14 +1303,12 @@
       <c r="C5" s="2">
         <v>1050</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>14220</v>
@@ -1388,14 +1316,12 @@
       <c r="C6" s="2">
         <v>15021</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>6707</v>
@@ -1403,14 +1329,12 @@
       <c r="C7" s="2">
         <v>7208</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D7" s="2"/>
       <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>8881</v>
@@ -1418,14 +1342,12 @@
       <c r="C8" s="2">
         <v>7624</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>6009</v>
@@ -1433,14 +1355,12 @@
       <c r="C9" s="2">
         <v>7128</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>10926</v>
@@ -1448,14 +1368,12 @@
       <c r="C10" s="2">
         <v>12071</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>13614</v>
@@ -1463,14 +1381,12 @@
       <c r="C11" s="2">
         <v>18163</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>8116</v>
@@ -1478,14 +1394,12 @@
       <c r="C12" s="2">
         <v>11704</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>9725</v>
@@ -1493,14 +1407,12 @@
       <c r="C13" s="2">
         <v>8949</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>665</v>
@@ -1515,7 +1427,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>775</v>
@@ -1523,14 +1435,12 @@
       <c r="C15" s="2">
         <v>871</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="16"/>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>1600</v>
@@ -1538,14 +1448,12 @@
       <c r="C16" s="2">
         <v>1291</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>1309</v>
@@ -1553,14 +1461,12 @@
       <c r="C17" s="2">
         <v>1010</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D17" s="2"/>
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>4160</v>
@@ -1568,14 +1474,12 @@
       <c r="C18" s="2">
         <v>4159</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D18" s="2"/>
       <c r="E18" s="16"/>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>1018</v>
@@ -1583,9 +1487,7 @@
       <c r="C19" s="2">
         <v>1050</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>
@@ -1598,7 +1500,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,19 +1510,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -1633,14 +1535,12 @@
       <c r="C2" s="2">
         <v>1349</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>1201</v>
@@ -1648,14 +1548,12 @@
       <c r="C3" s="2">
         <v>1055</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>4246</v>
@@ -1663,14 +1561,12 @@
       <c r="C4" s="2">
         <v>4132</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>1150</v>
@@ -1678,14 +1574,12 @@
       <c r="C5" s="2">
         <v>1162</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>14044</v>
@@ -1693,14 +1587,12 @@
       <c r="C6" s="2">
         <v>15204</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>7102</v>
@@ -1715,7 +1607,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>8612</v>
@@ -1730,7 +1622,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>6443</v>
@@ -1738,14 +1630,12 @@
       <c r="C9" s="2">
         <v>7386</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>10992</v>
@@ -1753,14 +1643,12 @@
       <c r="C10" s="2">
         <v>12196</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>13733</v>
@@ -1768,14 +1656,12 @@
       <c r="C11" s="2">
         <v>18336</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>7964</v>
@@ -1783,14 +1669,12 @@
       <c r="C12" s="2">
         <v>11648</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>9843</v>
@@ -1798,14 +1682,12 @@
       <c r="C13" s="2">
         <v>9083</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>651</v>
@@ -1820,7 +1702,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>759</v>
@@ -1835,7 +1717,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>360</v>
@@ -1843,14 +1725,12 @@
       <c r="C16" s="2">
         <v>520</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>509</v>
@@ -1865,7 +1745,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>7793</v>
@@ -1880,7 +1760,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>6250</v>
@@ -1888,9 +1768,7 @@
       <c r="C19" s="2">
         <v>6378</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>
@@ -1902,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D414BD08-B070-48B1-A67D-E60E6639B344}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,24 +1791,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>28.3</v>
@@ -1938,14 +1816,12 @@
       <c r="C2" s="5">
         <v>32.299999999999997</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5">
         <v>96.6</v>
@@ -1953,9 +1829,7 @@
       <c r="C3" s="5">
         <v>93.5</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="16"/>
     </row>
   </sheetData>
@@ -1968,7 +1842,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1978,24 +1852,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>26.7</v>
@@ -2010,7 +1884,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5">
         <v>96</v>
@@ -2018,9 +1892,7 @@
       <c r="C3" s="5">
         <v>93.8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="16"/>
     </row>
   </sheetData>
@@ -2033,7 +1905,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,24 +1915,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>29.2</v>
@@ -2075,7 +1947,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5">
         <v>95.1</v>
@@ -2083,9 +1955,7 @@
       <c r="C3" s="5">
         <v>95.8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="16"/>
     </row>
   </sheetData>
@@ -2108,24 +1978,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5">
         <v>27.8</v>
@@ -2140,7 +2010,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5">
         <v>61.9</v>
@@ -2155,7 +2025,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5">
         <v>28</v>
@@ -2170,7 +2040,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="5">
         <v>16</v>
@@ -2185,7 +2055,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5">
         <v>35.200000000000003</v>
@@ -2200,7 +2070,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="5">
         <v>63.6</v>
@@ -2215,7 +2085,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="5">
         <v>33.799999999999997</v>
@@ -2230,7 +2100,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5">
         <v>21.2</v>
@@ -2245,7 +2115,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="5">
         <v>34.299999999999997</v>
@@ -2260,7 +2130,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5">
         <v>59.9</v>
@@ -2275,7 +2145,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="5">
         <v>32.1</v>
@@ -2290,7 +2160,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5">
         <v>19.600000000000001</v>
@@ -2323,24 +2193,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5">
         <v>28.7</v>
@@ -2355,7 +2225,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5">
         <v>66.3</v>
@@ -2370,7 +2240,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5">
         <v>32.799999999999997</v>
@@ -2385,7 +2255,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="5">
         <v>16</v>
@@ -2400,7 +2270,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5">
         <v>37.1</v>
@@ -2415,7 +2285,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="5">
         <v>67</v>
@@ -2430,7 +2300,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="5">
         <v>40.9</v>
@@ -2445,7 +2315,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5">
         <v>22.4</v>
@@ -2460,7 +2330,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="5">
         <v>27.6</v>
@@ -2475,7 +2345,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5">
         <v>64.099999999999994</v>
@@ -2490,7 +2360,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="5">
         <v>38.9</v>
@@ -2505,7 +2375,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5">
         <v>20.2</v>
@@ -2538,24 +2408,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5">
         <v>30.9</v>
@@ -2570,7 +2440,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="5">
         <v>67.400000000000006</v>
@@ -2585,7 +2455,7 @@
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5">
         <v>30.3</v>
@@ -2600,7 +2470,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B5" s="5">
         <v>15.4</v>
@@ -2615,7 +2485,7 @@
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="5">
         <v>33.1</v>
@@ -2630,7 +2500,7 @@
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="5">
         <v>69.7</v>
@@ -2645,7 +2515,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B8" s="5">
         <v>38.6</v>
@@ -2660,7 +2530,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" s="5">
         <v>19.8</v>
@@ -2675,7 +2545,7 @@
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B10" s="5">
         <v>31.5</v>
@@ -2690,7 +2560,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B11" s="5">
         <v>65.400000000000006</v>
@@ -2705,7 +2575,7 @@
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B12" s="5">
         <v>36.6</v>
@@ -2720,7 +2590,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B13" s="5">
         <v>19.2</v>
@@ -2753,24 +2623,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5">
         <v>6.5</v>
@@ -2785,7 +2655,7 @@
     </row>
     <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5">
         <v>88.9</v>
@@ -2808,7 +2678,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,19 +2688,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2843,14 +2713,12 @@
       <c r="C2" s="2">
         <v>80570</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>33636</v>
@@ -2858,14 +2726,12 @@
       <c r="C3" s="2">
         <v>133033</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>15374</v>
@@ -2873,14 +2739,12 @@
       <c r="C4" s="2">
         <v>16302</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>4418</v>
@@ -2888,14 +2752,12 @@
       <c r="C5" s="2">
         <v>8749</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>200313</v>
@@ -2903,14 +2765,12 @@
       <c r="C6" s="2">
         <v>147320</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>99496</v>
@@ -2925,7 +2785,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>52196</v>
@@ -2940,7 +2800,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>17119</v>
@@ -2948,14 +2808,12 @@
       <c r="C9" s="2">
         <v>15088</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>280779</v>
@@ -2963,14 +2821,12 @@
       <c r="C10" s="2">
         <v>202807</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>108451</v>
@@ -2978,14 +2834,12 @@
       <c r="C11" s="2">
         <v>71262</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>41394</v>
@@ -2993,14 +2847,12 @@
       <c r="C12" s="2">
         <v>37668</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>130934</v>
@@ -3008,14 +2860,12 @@
       <c r="C13" s="2">
         <v>93877</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>389149</v>
@@ -3030,7 +2880,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>11116</v>
@@ -3045,7 +2895,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>15978</v>
@@ -3053,14 +2903,12 @@
       <c r="C16" s="2">
         <v>21534</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>27493</v>
@@ -3075,7 +2923,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>20181</v>
@@ -3090,7 +2938,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>11206</v>
@@ -3098,9 +2946,7 @@
       <c r="C19" s="2">
         <v>8371</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="14"/>
     </row>
   </sheetData>
@@ -3124,24 +2970,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="5">
         <v>9.1999999999999993</v>
@@ -3156,7 +3002,7 @@
     </row>
     <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="5">
         <v>91</v>
@@ -3189,24 +3035,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" s="10">
         <v>8.1999999999999993</v>
@@ -3221,7 +3067,7 @@
     </row>
     <row r="3" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" s="10">
         <v>92.1</v>
@@ -3244,7 +3090,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3254,24 +3100,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5">
         <v>2377.1</v>
@@ -3279,14 +3125,12 @@
       <c r="C2" s="5">
         <v>2377.1</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5">
         <v>1394.9</v>
@@ -3294,14 +3138,12 @@
       <c r="C3" s="5">
         <v>1394.9</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5">
         <v>58.7</v>
@@ -3309,14 +3151,12 @@
       <c r="C4" s="5">
         <v>58.7</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5">
         <v>554.1</v>
@@ -3324,14 +3164,12 @@
       <c r="C5" s="5">
         <v>591.5</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5">
         <v>147.9</v>
@@ -3339,14 +3177,12 @@
       <c r="C6" s="5">
         <v>140.69999999999999</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5">
         <v>19</v>
@@ -3361,7 +3197,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5">
         <v>1042.0999999999999</v>
@@ -3369,14 +3205,12 @@
       <c r="C8" s="5">
         <v>1068.5</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="5">
         <v>104.5</v>
@@ -3384,14 +3218,12 @@
       <c r="C9" s="5">
         <v>129.4</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="5">
         <v>10.6</v>
@@ -3399,9 +3231,7 @@
       <c r="C10" s="5">
         <v>13.8</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="3"/>
     </row>
   </sheetData>
@@ -3414,7 +3244,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3424,24 +3254,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5">
         <v>2377.1</v>
@@ -3449,14 +3279,12 @@
       <c r="C2" s="5">
         <v>2377.1</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5">
         <v>1436.6</v>
@@ -3464,14 +3292,12 @@
       <c r="C3" s="5">
         <v>1339.8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5">
         <v>60.4</v>
@@ -3479,14 +3305,12 @@
       <c r="C4" s="5">
         <v>56.4</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5">
         <v>592.4</v>
@@ -3494,14 +3318,12 @@
       <c r="C5" s="5">
         <v>545.29999999999995</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5">
         <v>131.6</v>
@@ -3509,14 +3331,12 @@
       <c r="C6" s="5">
         <v>132.1</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5">
         <v>24.4</v>
@@ -3531,7 +3351,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5">
         <v>1111.8</v>
@@ -3539,14 +3359,12 @@
       <c r="C8" s="5">
         <v>989.3</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="5">
         <v>96.1</v>
@@ -3554,14 +3372,12 @@
       <c r="C9" s="5">
         <v>113.4</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="5">
         <v>10</v>
@@ -3569,9 +3385,7 @@
       <c r="C10" s="5">
         <v>9.4</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="3"/>
     </row>
   </sheetData>
@@ -3583,8 +3397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D73F7A61-89C3-46F7-B33E-BD073BCC0D50}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3594,24 +3408,24 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5">
         <v>2377.1</v>
@@ -3619,14 +3433,12 @@
       <c r="C2" s="5">
         <v>2377.1</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5">
         <v>1402</v>
@@ -3634,14 +3446,12 @@
       <c r="C3" s="5">
         <v>1393.2</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4" s="5">
         <v>59</v>
@@ -3649,15 +3459,13 @@
       <c r="C4" s="5">
         <v>58.6</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="3"/>
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B5" s="5">
         <v>555.9</v>
@@ -3665,14 +3473,12 @@
       <c r="C5" s="5">
         <v>544.6</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5">
         <v>135.19999999999999</v>
@@ -3680,14 +3486,12 @@
       <c r="C6" s="5">
         <v>133</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="5">
         <v>27.1</v>
@@ -3702,7 +3506,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="5">
         <v>1067.2</v>
@@ -3710,14 +3514,12 @@
       <c r="C8" s="5">
         <v>1013.9</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D8" s="5"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="5">
         <v>94.7</v>
@@ -3725,14 +3527,12 @@
       <c r="C9" s="5">
         <v>125.1</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="5">
         <v>10.1</v>
@@ -3740,9 +3540,7 @@
       <c r="C10" s="5">
         <v>12.8</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="5"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25"/>
@@ -3756,7 +3554,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3766,19 +3564,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -3796,7 +3594,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>37469</v>
@@ -3804,14 +3602,12 @@
       <c r="C3" s="2">
         <v>139793</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>15840</v>
@@ -3819,14 +3615,12 @@
       <c r="C4" s="2">
         <v>16517</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>3495</v>
@@ -3834,14 +3628,12 @@
       <c r="C5" s="2">
         <v>8482</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="14"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>186204</v>
@@ -3849,14 +3641,12 @@
       <c r="C6" s="2">
         <v>152470</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="14"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>97771</v>
@@ -3871,7 +3661,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>56442</v>
@@ -3886,7 +3676,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>40424</v>
@@ -3894,14 +3684,12 @@
       <c r="C9" s="2">
         <v>19245</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="14"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>259505</v>
@@ -3909,14 +3697,12 @@
       <c r="C10" s="2">
         <v>213322</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="14"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>96434</v>
@@ -3924,14 +3710,12 @@
       <c r="C11" s="2">
         <v>73554</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>36598</v>
@@ -3939,14 +3723,12 @@
       <c r="C12" s="2">
         <v>37511</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="14"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>126472</v>
@@ -3954,14 +3736,12 @@
       <c r="C13" s="2">
         <v>102257</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>362439</v>
@@ -3976,7 +3756,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>10872</v>
@@ -3991,7 +3771,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>15144</v>
@@ -3999,14 +3779,12 @@
       <c r="C16" s="2">
         <v>19545</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="14"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>26996</v>
@@ -4021,7 +3799,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>18721</v>
@@ -4036,7 +3814,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>10914</v>
@@ -4044,9 +3822,7 @@
       <c r="C19" s="2">
         <v>10373</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="14"/>
     </row>
   </sheetData>
@@ -4059,7 +3835,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4069,19 +3845,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4094,14 +3870,12 @@
       <c r="C2" s="2">
         <v>72918</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>33295</v>
@@ -4109,14 +3883,12 @@
       <c r="C3" s="2">
         <v>136124</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>14507</v>
@@ -4124,14 +3896,12 @@
       <c r="C4" s="2">
         <v>15077</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>4187</v>
@@ -4139,14 +3909,12 @@
       <c r="C5" s="2">
         <v>8122</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>41160</v>
@@ -4154,14 +3922,12 @@
       <c r="C6" s="2">
         <v>46509</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>89427</v>
@@ -4176,7 +3942,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>51516</v>
@@ -4191,7 +3957,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>14450</v>
@@ -4199,14 +3965,12 @@
       <c r="C9" s="2">
         <v>14565</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>99876</v>
@@ -4214,14 +3978,12 @@
       <c r="C10" s="2">
         <v>79107</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>35735</v>
@@ -4229,14 +3991,12 @@
       <c r="C11" s="2">
         <v>22089</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>14980</v>
@@ -4244,14 +4004,12 @@
       <c r="C12" s="2">
         <v>11337</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>49161</v>
@@ -4259,14 +4017,12 @@
       <c r="C13" s="2">
         <v>45681</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>362199</v>
@@ -4281,7 +4037,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>10530</v>
@@ -4296,7 +4052,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>14609</v>
@@ -4304,14 +4060,12 @@
       <c r="C16" s="2">
         <v>21292</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>24677</v>
@@ -4326,7 +4080,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>18246</v>
@@ -4341,7 +4095,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>4778</v>
@@ -4349,9 +4103,7 @@
       <c r="C19" s="2">
         <v>4978</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>
@@ -4364,7 +4116,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4374,19 +4126,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4399,14 +4151,12 @@
       <c r="C2" s="2">
         <v>80570</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>33636</v>
@@ -4414,14 +4164,12 @@
       <c r="C3" s="2">
         <v>133033</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>15374</v>
@@ -4429,14 +4177,12 @@
       <c r="C4" s="2">
         <v>16302</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>4418</v>
@@ -4444,14 +4190,12 @@
       <c r="C5" s="2">
         <v>8749</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>42284</v>
@@ -4459,14 +4203,12 @@
       <c r="C6" s="2">
         <v>47837</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>99496</v>
@@ -4481,7 +4223,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>52196</v>
@@ -4496,7 +4238,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>15612</v>
@@ -4504,14 +4246,12 @@
       <c r="C9" s="2">
         <v>15017</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>105474</v>
@@ -4519,14 +4259,12 @@
       <c r="C10" s="2">
         <v>82137</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>38916</v>
@@ -4534,14 +4272,12 @@
       <c r="C11" s="2">
         <v>24193</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>15345</v>
@@ -4549,14 +4285,12 @@
       <c r="C12" s="2">
         <v>12174</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>51213</v>
@@ -4564,14 +4298,12 @@
       <c r="C13" s="2">
         <v>45770</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>389149</v>
@@ -4586,7 +4318,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>11116</v>
@@ -4601,7 +4333,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>15978</v>
@@ -4609,14 +4341,12 @@
       <c r="C16" s="2">
         <v>21534</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>27493</v>
@@ -4631,7 +4361,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>20181</v>
@@ -4646,7 +4376,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>4599</v>
@@ -4654,9 +4384,7 @@
       <c r="C19" s="2">
         <v>4429</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>
@@ -4669,7 +4397,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4679,19 +4407,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -4704,14 +4432,12 @@
       <c r="C2" s="2">
         <v>81282</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>37469</v>
@@ -4719,14 +4445,12 @@
       <c r="C3" s="2">
         <v>139792</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>15779</v>
@@ -4734,14 +4458,12 @@
       <c r="C4" s="2">
         <v>16474</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>3495</v>
@@ -4749,14 +4471,12 @@
       <c r="C5" s="2">
         <v>8482</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>45418</v>
@@ -4764,14 +4484,12 @@
       <c r="C6" s="2">
         <v>48494</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>97767</v>
@@ -4786,7 +4504,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>56442</v>
@@ -4801,7 +4519,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>13231</v>
@@ -4809,14 +4527,12 @@
       <c r="C9" s="2">
         <v>15928</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>108476</v>
@@ -4824,14 +4540,12 @@
       <c r="C10" s="2">
         <v>83314</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>39729</v>
@@ -4839,14 +4553,12 @@
       <c r="C11" s="2">
         <v>24565</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>15927</v>
@@ -4854,14 +4566,12 @@
       <c r="C12" s="2">
         <v>12513</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>52820</v>
@@ -4869,14 +4579,12 @@
       <c r="C13" s="2">
         <v>46236</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2">
         <v>362438</v>
@@ -4891,7 +4599,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>10872</v>
@@ -4906,7 +4614,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>15118</v>
@@ -4914,14 +4622,12 @@
       <c r="C16" s="2">
         <v>19545</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>26996</v>
@@ -4936,7 +4642,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>18298</v>
@@ -4951,7 +4657,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>3402</v>
@@ -4959,9 +4665,7 @@
       <c r="C19" s="2">
         <v>4213</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>
@@ -4974,29 +4678,30 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5009,14 +4714,12 @@
       <c r="C2" s="2">
         <v>94634</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>42231</v>
@@ -5024,14 +4727,12 @@
       <c r="C3" s="2">
         <v>128258</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>52225</v>
@@ -5039,14 +4740,12 @@
       <c r="C4" s="2">
         <v>64279</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>4138</v>
@@ -5054,14 +4753,12 @@
       <c r="C5" s="2">
         <v>8673</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>578545</v>
@@ -5069,14 +4766,12 @@
       <c r="C6" s="2">
         <v>701037</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>635007</v>
@@ -5091,7 +4786,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>427471</v>
@@ -5106,7 +4801,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>85414</v>
@@ -5114,14 +4809,12 @@
       <c r="C9" s="2">
         <v>102628</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>1100082</v>
@@ -5129,14 +4822,12 @@
       <c r="C10" s="2">
         <v>931991</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>502972</v>
@@ -5144,14 +4835,12 @@
       <c r="C11" s="2">
         <v>410259</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>120868</v>
@@ -5159,14 +4848,12 @@
       <c r="C12" s="2">
         <v>138090</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>476241</v>
@@ -5174,14 +4861,12 @@
       <c r="C13" s="2">
         <v>383641</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>226570</v>
@@ -5196,7 +4881,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>7933</v>
@@ -5211,7 +4896,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>5762</v>
@@ -5219,14 +4904,12 @@
       <c r="C16" s="2">
         <v>10542</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>12284</v>
@@ -5241,7 +4924,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>160114</v>
@@ -5256,7 +4939,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>23542</v>
@@ -5264,9 +4947,7 @@
       <c r="C19" s="2">
         <v>24830</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>
@@ -5279,29 +4960,30 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5314,14 +4996,12 @@
       <c r="C2" s="2">
         <v>104041</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>44039</v>
@@ -5329,14 +5009,12 @@
       <c r="C3" s="2">
         <v>134331</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>63950</v>
@@ -5344,14 +5022,12 @@
       <c r="C4" s="2">
         <v>67808</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>4500</v>
@@ -5359,14 +5035,12 @@
       <c r="C5" s="2">
         <v>9184</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>601291</v>
@@ -5374,14 +5048,12 @@
       <c r="C6" s="2">
         <v>718584</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>667346</v>
@@ -5396,7 +5068,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>463562</v>
@@ -5411,7 +5083,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>93819</v>
@@ -5419,14 +5091,12 @@
       <c r="C9" s="2">
         <v>107037</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>1152365</v>
@@ -5434,14 +5104,12 @@
       <c r="C10" s="2">
         <v>991501</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>529788</v>
@@ -5449,14 +5117,12 @@
       <c r="C11" s="2">
         <v>439405</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>124546</v>
@@ -5464,14 +5130,12 @@
       <c r="C12" s="2">
         <v>142487</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>498031</v>
@@ -5479,14 +5143,12 @@
       <c r="C13" s="2">
         <v>409609</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>258851</v>
@@ -5501,7 +5163,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>8617</v>
@@ -5516,7 +5178,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>6313</v>
@@ -5524,14 +5186,12 @@
       <c r="C16" s="2">
         <v>10763</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>14237</v>
@@ -5546,7 +5206,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>159669</v>
@@ -5561,7 +5221,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>25275</v>
@@ -5569,9 +5229,7 @@
       <c r="C19" s="2">
         <v>25340</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>
@@ -5584,29 +5242,30 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E19"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -5619,14 +5278,12 @@
       <c r="C2" s="2">
         <v>109615</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D2" s="2"/>
       <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
         <v>45016</v>
@@ -5634,14 +5291,12 @@
       <c r="C3" s="2">
         <v>147411</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2">
         <v>67002</v>
@@ -5649,14 +5304,12 @@
       <c r="C4" s="2">
         <v>68072</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
         <v>4019</v>
@@ -5664,14 +5317,12 @@
       <c r="C5" s="2">
         <v>9858</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
         <v>637856</v>
@@ -5679,14 +5330,12 @@
       <c r="C6" s="2">
         <v>737284</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>694320</v>
@@ -5701,7 +5350,7 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
         <v>486075</v>
@@ -5716,7 +5365,7 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>85245</v>
@@ -5724,14 +5373,12 @@
       <c r="C9" s="2">
         <v>117647</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D9" s="2"/>
       <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
         <v>1192331</v>
@@ -5739,14 +5386,12 @@
       <c r="C10" s="2">
         <v>1016137</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
         <v>545588</v>
@@ -5754,14 +5399,12 @@
       <c r="C11" s="2">
         <v>450427</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D11" s="2"/>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
         <v>126838</v>
@@ -5769,14 +5412,12 @@
       <c r="C12" s="2">
         <v>145753</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D12" s="2"/>
       <c r="E12" s="16"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>519904</v>
@@ -5784,14 +5425,12 @@
       <c r="C13" s="2">
         <v>419956</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D13" s="2"/>
       <c r="E13" s="16"/>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
         <v>235818</v>
@@ -5806,7 +5445,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2">
         <v>8247</v>
@@ -5821,7 +5460,7 @@
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2">
         <v>5445</v>
@@ -5829,14 +5468,12 @@
       <c r="C16" s="2">
         <v>10172</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
         <v>13741</v>
@@ -5851,7 +5488,7 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="2">
         <v>142604</v>
@@ -5866,7 +5503,7 @@
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2">
         <v>21261</v>
@@ -5874,9 +5511,7 @@
       <c r="C19" s="2">
         <v>26872</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D19" s="2"/>
       <c r="E19" s="16"/>
     </row>
   </sheetData>

</xml_diff>